<commit_message>
add grafico de linha
</commit_message>
<xml_diff>
--- a/dados climaticos.xlsx
+++ b/dados climaticos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>Dia</t>
   </si>
@@ -64,40 +64,34 @@
     <t>23/12/2024</t>
   </si>
   <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>97</t>
-  </si>
-  <si>
-    <t>98</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>70</t>
-  </si>
-  <si>
-    <t>65</t>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>55</t>
   </si>
   <si>
     <t>50</t>
@@ -495,13 +489,13 @@
         <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
         <v>23</v>
-      </c>
-      <c r="F2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -512,16 +506,10 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -535,13 +523,13 @@
         <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
         <v>24</v>
-      </c>
-      <c r="F4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -558,10 +546,10 @@
         <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -572,16 +560,16 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
         <v>22</v>
       </c>
-      <c r="E6" t="s">
-        <v>25</v>
-      </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>